<commit_message>
update report and folder structure
</commit_message>
<xml_diff>
--- a/wdis_of_interest.xlsx
+++ b/wdis_of_interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/gulacsy_dominik_student_ceu_edu/Documents/1st_trimester/DE2/DE2_Term_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_AD4D6204247ACDAA4110B463E9D4E2FA693EDF13" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4A8E297E-A8E7-4872-ABD8-4C359EDF5360}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_AD4D6204247ACDAA4110B463E9D4E2FA693EDF13" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D49E8F0-0C99-4EB3-8B50-7ACD32C4211E}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WDI" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>wdi</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Population</t>
+  </si>
+  <si>
+    <t>SI.POV.GINI</t>
+  </si>
+  <si>
+    <t>Gini index (World Bank estimate)</t>
+  </si>
+  <si>
+    <t>SE.XPD.TOTL.GD.ZS</t>
+  </si>
+  <si>
+    <t>Government expenditure on education, total (% of GDP)</t>
   </si>
 </sst>
 </file>
@@ -133,14 +145,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +530,22 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://data.worldbank.org/indicator/SH.PRV.SMOK.FE?view=chart" xr:uid="{C22ED365-FDFE-444B-BAB8-C7BF6F14CE3C}"/>
@@ -523,7 +554,10 @@
     <hyperlink ref="A6" r:id="rId4" display="https://data.worldbank.org/indicator/SL.UEM.TOTL.FE.ZS?view=chart" xr:uid="{B922D21B-C820-4DAE-BD50-80A2419508CD}"/>
     <hyperlink ref="A5" r:id="rId5" display="https://data.worldbank.org/indicator/SH.ALC.PCAP.FE.LI?view=chart" xr:uid="{65E84A87-C646-42DF-9A28-EC12DF00AA95}"/>
     <hyperlink ref="A4" r:id="rId6" display="https://data.worldbank.org/indicator/SH.ALC.PCAP.MA.LI?view=chart" xr:uid="{AC1B5FD0-2E23-4B4D-B380-2D6ACE27B71A}"/>
+    <hyperlink ref="A9" r:id="rId7" display="https://data.worldbank.org/indicator/SI.POV.GINI" xr:uid="{FC4A9CC9-0C7F-4C85-BD6F-1F1CDB233A73}"/>
+    <hyperlink ref="A10" r:id="rId8" display="https://data.worldbank.org/indicator/SE.XPD.TOTL.GD.ZS" xr:uid="{F14748EC-7AAE-4C33-9300-64092BCDD2EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>